<commit_message>
Clean up misc., update excel files
</commit_message>
<xml_diff>
--- a/docs/public/help/help_linked_docs/accessioning_template_extended.xlsx
+++ b/docs/public/help/help_linked_docs/accessioning_template_extended.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drioux/Documents/help_linked_docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drioux/CGAP/cgap-portal/docs/public/help/help_linked_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8759A513-8D9E-A648-957E-C89592E7EB8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F09799-89AA-1540-9465-8D3A56AF573D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3140" windowWidth="28800" windowHeight="14860" xr2:uid="{FB0E66EA-1423-4875-8AFB-50DDC911B1EB}"/>
+    <workbookView xWindow="140" yWindow="880" windowWidth="28800" windowHeight="14860" xr2:uid="{FB0E66EA-1423-4875-8AFB-50DDC911B1EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Accession data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,20 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="71">
-  <si>
-    <t>Other ID</t>
-  </si>
-  <si>
-    <t>place holder for other pt IDs</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="74">
   <si>
     <t>dd/mm/yyyy</t>
   </si>
   <si>
-    <t>M or F</t>
-  </si>
-  <si>
     <t xml:space="preserve">proband or relation to proband </t>
   </si>
   <si>
@@ -165,9 +156,6 @@
     <t>YYYY</t>
   </si>
   <si>
-    <t>WGS, WES, etc.</t>
-  </si>
-  <si>
     <t>Correction Notes</t>
   </si>
   <si>
@@ -222,22 +210,43 @@
     <t>Unique Analysis ID*</t>
   </si>
   <si>
-    <t>Pt ID generated manually or by barcode-</t>
-  </si>
-  <si>
-    <t>family ID generated manually or by barcode</t>
-  </si>
-  <si>
     <t>Files</t>
   </si>
   <si>
     <t>Family ID</t>
   </si>
   <si>
-    <t>Clinic Notes</t>
-  </si>
-  <si>
-    <t>Unique ID for patient for this analysis</t>
+    <t>Age Units</t>
+  </si>
+  <si>
+    <t>Case Files</t>
+  </si>
+  <si>
+    <t>Genome Build</t>
+  </si>
+  <si>
+    <t>ID for the analysis group</t>
+  </si>
+  <si>
+    <t>ID for sample specific to this analysis</t>
+  </si>
+  <si>
+    <t>Pt ID generated manually or by barcode</t>
+  </si>
+  <si>
+    <t>Family ID generated manually or by barcode</t>
+  </si>
+  <si>
+    <t>M, F, U</t>
+  </si>
+  <si>
+    <t>WGS, WES</t>
+  </si>
+  <si>
+    <t>Comma-separated</t>
+  </si>
+  <si>
+    <t>hg19, hg38</t>
   </si>
 </sst>
 </file>
@@ -315,7 +324,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -430,15 +439,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -529,11 +529,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -552,7 +594,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -574,48 +615,28 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -631,12 +652,50 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -961,28 +1020,30 @@
   <dimension ref="A1:CC4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="4"/>
-    <col min="2" max="2" width="12.6640625" style="7" customWidth="1"/>
-    <col min="3" max="10" width="12.6640625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="27.1640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" style="7" customWidth="1"/>
+    <col min="3" max="9" width="12.6640625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" style="7" customWidth="1"/>
     <col min="12" max="19" width="16" style="7" customWidth="1"/>
     <col min="20" max="20" width="14.5" style="4" customWidth="1"/>
     <col min="21" max="22" width="15.5" style="4" customWidth="1"/>
     <col min="23" max="23" width="14.33203125" style="4" customWidth="1"/>
-    <col min="24" max="24" width="16.5" style="4" customWidth="1"/>
-    <col min="25" max="25" width="12.6640625" style="6" customWidth="1"/>
+    <col min="24" max="24" width="16.5" style="6" customWidth="1"/>
+    <col min="25" max="25" width="12.6640625" style="7" customWidth="1"/>
     <col min="26" max="35" width="16" style="7" customWidth="1"/>
     <col min="36" max="37" width="14.5" style="4" customWidth="1"/>
     <col min="38" max="38" width="15.5" style="4" customWidth="1"/>
     <col min="39" max="39" width="14.33203125" style="4" customWidth="1"/>
     <col min="40" max="40" width="14.33203125" style="5" customWidth="1"/>
-    <col min="41" max="41" width="12.6640625" style="6" customWidth="1"/>
-    <col min="42" max="77" width="16" style="7" customWidth="1"/>
+    <col min="41" max="41" width="12.6640625" style="4" customWidth="1"/>
+    <col min="42" max="42" width="16" style="51" customWidth="1"/>
+    <col min="43" max="77" width="16" style="7" customWidth="1"/>
     <col min="78" max="78" width="14.5" style="4" customWidth="1"/>
     <col min="79" max="79" width="15.5" style="4" customWidth="1"/>
     <col min="80" max="80" width="14.33203125" style="4" customWidth="1"/>
@@ -991,219 +1052,221 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:81" s="3" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="43" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39"/>
-      <c r="T1" s="42"/>
-      <c r="U1" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="V1" s="39"/>
-      <c r="W1" s="39"/>
-      <c r="X1" s="39"/>
-      <c r="Y1" s="40"/>
-      <c r="Z1" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA1" s="39"/>
-      <c r="AB1" s="39"/>
-      <c r="AC1" s="39"/>
-      <c r="AD1" s="39"/>
-      <c r="AE1" s="39"/>
-      <c r="AF1" s="39"/>
-      <c r="AG1" s="39"/>
-      <c r="AH1" s="39"/>
-      <c r="AI1" s="39"/>
-      <c r="AJ1" s="39"/>
-      <c r="AK1" s="39"/>
-      <c r="AL1" s="39"/>
-      <c r="AM1" s="39"/>
-      <c r="AN1" s="39"/>
-      <c r="AO1" s="40"/>
-      <c r="AP1" s="16"/>
-      <c r="AQ1" s="16"/>
-      <c r="AR1" s="16"/>
-      <c r="AS1" s="16"/>
-      <c r="AT1" s="16"/>
-      <c r="AU1" s="16"/>
-      <c r="AV1" s="16"/>
-      <c r="AW1" s="16"/>
-      <c r="AX1" s="16"/>
-      <c r="AY1" s="16"/>
-      <c r="AZ1" s="16"/>
-      <c r="BA1" s="16"/>
-      <c r="BB1" s="16"/>
-      <c r="BC1" s="16"/>
-      <c r="BD1" s="16"/>
-      <c r="BE1" s="16"/>
-      <c r="BF1" s="16"/>
-      <c r="BG1" s="16"/>
-      <c r="BH1" s="16"/>
-      <c r="BI1" s="16"/>
-      <c r="BJ1" s="16"/>
-      <c r="BK1" s="16"/>
-      <c r="BL1" s="16"/>
-      <c r="BM1" s="16"/>
-      <c r="BN1" s="16"/>
-      <c r="BO1" s="16"/>
-      <c r="BP1" s="16"/>
-      <c r="BQ1" s="16"/>
-      <c r="BR1" s="16"/>
-      <c r="BS1" s="16"/>
-      <c r="BT1" s="16"/>
-      <c r="BU1" s="16"/>
-      <c r="BV1" s="16"/>
-      <c r="BW1" s="16"/>
-      <c r="BX1" s="16"/>
-      <c r="BY1" s="16"/>
-      <c r="BZ1" s="17"/>
-      <c r="CA1" s="17"/>
-      <c r="CB1" s="17"/>
-      <c r="CC1" s="17"/>
+      <c r="A1" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AJ1" s="30"/>
+      <c r="AK1" s="30"/>
+      <c r="AL1" s="30"/>
+      <c r="AM1" s="30"/>
+      <c r="AN1" s="30"/>
+      <c r="AO1" s="36"/>
+      <c r="AP1" s="37"/>
+      <c r="AQ1" s="15"/>
+      <c r="AR1" s="15"/>
+      <c r="AS1" s="15"/>
+      <c r="AT1" s="15"/>
+      <c r="AU1" s="15"/>
+      <c r="AV1" s="15"/>
+      <c r="AW1" s="15"/>
+      <c r="AX1" s="15"/>
+      <c r="AY1" s="15"/>
+      <c r="AZ1" s="15"/>
+      <c r="BA1" s="15"/>
+      <c r="BB1" s="15"/>
+      <c r="BC1" s="15"/>
+      <c r="BD1" s="15"/>
+      <c r="BE1" s="15"/>
+      <c r="BF1" s="15"/>
+      <c r="BG1" s="15"/>
+      <c r="BH1" s="15"/>
+      <c r="BI1" s="15"/>
+      <c r="BJ1" s="15"/>
+      <c r="BK1" s="15"/>
+      <c r="BL1" s="15"/>
+      <c r="BM1" s="15"/>
+      <c r="BN1" s="15"/>
+      <c r="BO1" s="15"/>
+      <c r="BP1" s="15"/>
+      <c r="BQ1" s="15"/>
+      <c r="BR1" s="15"/>
+      <c r="BS1" s="15"/>
+      <c r="BT1" s="15"/>
+      <c r="BU1" s="15"/>
+      <c r="BV1" s="15"/>
+      <c r="BW1" s="15"/>
+      <c r="BX1" s="15"/>
+      <c r="BY1" s="15"/>
+      <c r="BZ1" s="16"/>
+      <c r="CA1" s="16"/>
+      <c r="CB1" s="16"/>
+      <c r="CC1" s="16"/>
     </row>
     <row r="2" spans="1:81" s="9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="K2" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="L2" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="R2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="T2" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="U2" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="V2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="W2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="X2" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y2" s="52" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z2" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA2" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB2" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC2" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD2" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE2" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF2" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG2" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH2" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="AI2" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ2" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="AK2" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL2" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM2" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN2" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="AO2" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="K2" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="P2" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q2" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="R2" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="S2" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="T2" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="U2" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="V2" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="W2" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="X2" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y2" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z2" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA2" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB2" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC2" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="AD2" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="AE2" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF2" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG2" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="AH2" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="AI2" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="AJ2" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="AK2" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="AL2" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM2" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="AN2" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="AO2" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="AP2" s="2"/>
+      <c r="AP2" s="41" t="s">
+        <v>65</v>
+      </c>
       <c r="AQ2" s="2"/>
       <c r="AR2" s="2"/>
       <c r="AS2" s="2"/>
@@ -1244,202 +1307,252 @@
       <c r="CB2" s="1"/>
       <c r="CC2" s="1"/>
     </row>
-    <row r="3" spans="1:81" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+    <row r="3" spans="1:81" s="47" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="B3" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" s="29" t="s">
+      <c r="I3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="29"/>
-      <c r="F3" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" s="30"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32" t="s">
+      <c r="J3" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="32" t="s">
+      <c r="K3" s="49"/>
+      <c r="L3" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q3" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="R3" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="S3" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="T3" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="P3" s="32" t="s">
+      <c r="U3" s="26"/>
+      <c r="V3" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="W3" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="X3" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="Q3" s="32" t="s">
+      <c r="Y3" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z3" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA3" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="R3" s="32" t="s">
+      <c r="AB3" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC3" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE3" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF3" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG3" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH3" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI3" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="S3" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="T3" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="U3" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="V3" s="33"/>
-      <c r="W3" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="X3" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y3" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z3" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA3" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB3" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC3" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="AD3" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE3" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="AF3" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="AG3" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="AH3" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="AI3" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="AJ3" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK3" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL3" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="AM3" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="AN3" s="37"/>
-      <c r="AO3" s="31"/>
-      <c r="AP3" s="10"/>
-      <c r="AQ3" s="10"/>
-      <c r="AR3" s="10"/>
-      <c r="AS3" s="10"/>
-      <c r="AT3" s="10"/>
-      <c r="AU3" s="10"/>
-      <c r="AV3" s="10"/>
-      <c r="AW3" s="10"/>
-      <c r="AX3" s="10"/>
-      <c r="AY3" s="10"/>
-      <c r="AZ3" s="10"/>
-      <c r="BA3" s="10"/>
-      <c r="BB3" s="10"/>
-      <c r="BC3" s="10"/>
-      <c r="BD3" s="10"/>
-      <c r="BE3" s="10"/>
-      <c r="BF3" s="10"/>
-      <c r="BG3" s="10"/>
-      <c r="BH3" s="10"/>
-      <c r="BI3" s="10"/>
-      <c r="BJ3" s="10"/>
-      <c r="BK3" s="10"/>
-      <c r="BL3" s="10"/>
-      <c r="BM3" s="10"/>
-      <c r="BN3" s="10"/>
-      <c r="BO3" s="10"/>
-      <c r="BP3" s="10"/>
-      <c r="BQ3" s="10"/>
-      <c r="BR3" s="10"/>
-      <c r="BS3" s="10"/>
-      <c r="BT3" s="10"/>
-      <c r="BU3" s="10"/>
-      <c r="BV3" s="10"/>
-      <c r="BW3" s="10"/>
-      <c r="BX3" s="10"/>
-      <c r="BY3" s="10"/>
+      <c r="AK3" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL3" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM3" s="28"/>
+      <c r="AN3" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO3" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="AP3" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="AQ3" s="46"/>
+      <c r="AR3" s="46"/>
+      <c r="AS3" s="46"/>
+      <c r="AT3" s="46"/>
+      <c r="AU3" s="46"/>
+      <c r="AV3" s="46"/>
+      <c r="AW3" s="46"/>
+      <c r="AX3" s="46"/>
+      <c r="AY3" s="46"/>
+      <c r="AZ3" s="46"/>
+      <c r="BA3" s="46"/>
+      <c r="BB3" s="46"/>
+      <c r="BC3" s="46"/>
+      <c r="BD3" s="46"/>
+      <c r="BE3" s="46"/>
+      <c r="BF3" s="46"/>
+      <c r="BG3" s="46"/>
+      <c r="BH3" s="46"/>
+      <c r="BI3" s="46"/>
+      <c r="BJ3" s="46"/>
+      <c r="BK3" s="46"/>
+      <c r="BL3" s="46"/>
+      <c r="BM3" s="46"/>
+      <c r="BN3" s="46"/>
+      <c r="BO3" s="46"/>
+      <c r="BP3" s="46"/>
+      <c r="BQ3" s="46"/>
+      <c r="BR3" s="46"/>
+      <c r="BS3" s="46"/>
+      <c r="BT3" s="46"/>
+      <c r="BU3" s="46"/>
+      <c r="BV3" s="46"/>
+      <c r="BW3" s="46"/>
+      <c r="BX3" s="46"/>
+      <c r="BY3" s="46"/>
+      <c r="BZ3" s="45"/>
+      <c r="CA3" s="45"/>
+      <c r="CB3" s="45"/>
+      <c r="CC3" s="45"/>
     </row>
     <row r="4" spans="1:81" x14ac:dyDescent="0.15">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27"/>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="27"/>
-      <c r="R4" s="27"/>
-      <c r="S4" s="27"/>
-      <c r="T4" s="26"/>
-      <c r="U4" s="26"/>
-      <c r="V4" s="26"/>
-      <c r="W4" s="26"/>
-      <c r="X4" s="26"/>
-      <c r="Y4" s="19"/>
-      <c r="Z4" s="27"/>
-      <c r="AA4" s="27"/>
-      <c r="AB4" s="27"/>
-      <c r="AC4" s="27"/>
-      <c r="AD4" s="27"/>
-      <c r="AE4" s="27"/>
-      <c r="AF4" s="27"/>
-      <c r="AG4" s="27"/>
-      <c r="AH4" s="27"/>
-      <c r="AI4" s="27"/>
-      <c r="AJ4" s="26"/>
-      <c r="AK4" s="26"/>
-      <c r="AL4" s="26"/>
-      <c r="AM4" s="26"/>
-      <c r="AN4" s="24"/>
-      <c r="AO4" s="19"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="22"/>
+      <c r="X4" s="17"/>
+      <c r="Y4" s="23"/>
+      <c r="Z4" s="23"/>
+      <c r="AA4" s="23"/>
+      <c r="AB4" s="23"/>
+      <c r="AC4" s="23"/>
+      <c r="AD4" s="23"/>
+      <c r="AE4" s="23"/>
+      <c r="AF4" s="23"/>
+      <c r="AG4" s="23"/>
+      <c r="AH4" s="23"/>
+      <c r="AI4" s="23"/>
+      <c r="AJ4" s="22"/>
+      <c r="AK4" s="22"/>
+      <c r="AL4" s="22"/>
+      <c r="AM4" s="22"/>
+      <c r="AN4" s="21"/>
+      <c r="AO4" s="22"/>
+      <c r="AP4" s="50"/>
+      <c r="AQ4" s="23"/>
+      <c r="AR4" s="23"/>
+      <c r="AS4" s="23"/>
+      <c r="AT4" s="23"/>
+      <c r="AU4" s="23"/>
+      <c r="AV4" s="23"/>
+      <c r="AW4" s="23"/>
+      <c r="AX4" s="23"/>
+      <c r="AY4" s="23"/>
+      <c r="AZ4" s="23"/>
+      <c r="BA4" s="23"/>
+      <c r="BB4" s="23"/>
+      <c r="BC4" s="23"/>
+      <c r="BD4" s="23"/>
+      <c r="BE4" s="23"/>
+      <c r="BF4" s="23"/>
+      <c r="BG4" s="23"/>
+      <c r="BH4" s="23"/>
+      <c r="BI4" s="23"/>
+      <c r="BJ4" s="23"/>
+      <c r="BK4" s="23"/>
+      <c r="BL4" s="23"/>
+      <c r="BM4" s="23"/>
+      <c r="BN4" s="23"/>
+      <c r="BO4" s="23"/>
+      <c r="BP4" s="23"/>
+      <c r="BQ4" s="23"/>
+      <c r="BR4" s="23"/>
+      <c r="BS4" s="23"/>
+      <c r="BT4" s="23"/>
+      <c r="BU4" s="23"/>
+      <c r="BV4" s="23"/>
+      <c r="BW4" s="23"/>
+      <c r="BX4" s="23"/>
+      <c r="BY4" s="23"/>
+      <c r="BZ4" s="22"/>
+      <c r="CA4" s="22"/>
+      <c r="CB4" s="22"/>
+      <c r="CC4" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="U1:Y1"/>
-    <mergeCell ref="Z1:AO1"/>
-    <mergeCell ref="L1:T1"/>
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="K1:S1"/>
+    <mergeCell ref="T1:X1"/>
+    <mergeCell ref="Y1:AP1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update docs and spreadsheets for BAM sample ID
</commit_message>
<xml_diff>
--- a/docs/public/help/help_linked_docs/accessioning_template_extended.xlsx
+++ b/docs/public/help/help_linked_docs/accessioning_template_extended.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drioux/CGAP/cgap-portal/docs/public/help/help_linked_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F09799-89AA-1540-9465-8D3A56AF573D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95890A0-8CCF-C148-8E8F-FF19BF7A2C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="880" windowWidth="28800" windowHeight="14860" xr2:uid="{FB0E66EA-1423-4875-8AFB-50DDC911B1EB}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="28800" windowHeight="14860" xr2:uid="{FB0E66EA-1423-4875-8AFB-50DDC911B1EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Accession data" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="75">
   <si>
     <t>dd/mm/yyyy</t>
   </si>
@@ -165,9 +165,6 @@
     <t>Age</t>
   </si>
   <si>
-    <t>Patient ID*</t>
-  </si>
-  <si>
     <t>Sex*</t>
   </si>
   <si>
@@ -247,6 +244,12 @@
   </si>
   <si>
     <t>hg19, hg38</t>
+  </si>
+  <si>
+    <t>BAM Sample ID</t>
+  </si>
+  <si>
+    <t>Individual ID*</t>
   </si>
 </sst>
 </file>
@@ -575,7 +578,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -637,33 +640,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -696,6 +672,27 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1020,7 +1017,7 @@
   <dimension ref="A1:CC4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1042,8 +1039,9 @@
     <col min="39" max="39" width="14.33203125" style="4" customWidth="1"/>
     <col min="40" max="40" width="14.33203125" style="5" customWidth="1"/>
     <col min="41" max="41" width="12.6640625" style="4" customWidth="1"/>
-    <col min="42" max="42" width="16" style="51" customWidth="1"/>
-    <col min="43" max="77" width="16" style="7" customWidth="1"/>
+    <col min="42" max="42" width="16" style="7" customWidth="1"/>
+    <col min="43" max="43" width="16" style="42" customWidth="1"/>
+    <col min="44" max="77" width="16" style="7" customWidth="1"/>
     <col min="78" max="78" width="14.5" style="4" customWidth="1"/>
     <col min="79" max="79" width="15.5" style="4" customWidth="1"/>
     <col min="80" max="80" width="14.33203125" style="4" customWidth="1"/>
@@ -1052,55 +1050,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:81" s="3" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="33"/>
-      <c r="T1" s="29" t="s">
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="48"/>
+      <c r="T1" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="32" t="s">
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="50"/>
+      <c r="Y1" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="Z1" s="30"/>
-      <c r="AA1" s="30"/>
-      <c r="AB1" s="30"/>
-      <c r="AC1" s="30"/>
-      <c r="AD1" s="30"/>
-      <c r="AE1" s="30"/>
-      <c r="AF1" s="30"/>
-      <c r="AG1" s="30"/>
-      <c r="AH1" s="30"/>
-      <c r="AI1" s="30"/>
-      <c r="AJ1" s="30"/>
-      <c r="AK1" s="30"/>
-      <c r="AL1" s="30"/>
-      <c r="AM1" s="30"/>
-      <c r="AN1" s="30"/>
-      <c r="AO1" s="36"/>
-      <c r="AP1" s="37"/>
-      <c r="AQ1" s="15"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="47"/>
+      <c r="AE1" s="47"/>
+      <c r="AF1" s="47"/>
+      <c r="AG1" s="47"/>
+      <c r="AH1" s="47"/>
+      <c r="AI1" s="47"/>
+      <c r="AJ1" s="47"/>
+      <c r="AK1" s="47"/>
+      <c r="AL1" s="47"/>
+      <c r="AM1" s="47"/>
+      <c r="AN1" s="47"/>
+      <c r="AO1" s="47"/>
+      <c r="AP1" s="47"/>
+      <c r="AQ1" s="50"/>
       <c r="AR1" s="15"/>
       <c r="AS1" s="15"/>
       <c r="AT1" s="15"/>
@@ -1142,43 +1140,43 @@
     </row>
     <row r="2" spans="1:81" s="9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>45</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>41</v>
       </c>
       <c r="H2" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="I2" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="J2" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="K2" s="48" t="s">
+      <c r="J2" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="K2" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="11" t="s">
         <v>53</v>
-      </c>
-      <c r="L2" s="48" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>54</v>
       </c>
       <c r="N2" s="11" t="s">
         <v>4</v>
@@ -1199,10 +1197,10 @@
         <v>39</v>
       </c>
       <c r="T2" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="U2" s="12" t="s">
         <v>55</v>
-      </c>
-      <c r="U2" s="12" t="s">
-        <v>56</v>
       </c>
       <c r="V2" s="12" t="s">
         <v>7</v>
@@ -1213,23 +1211,23 @@
       <c r="X2" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="Y2" s="52" t="s">
+      <c r="Y2" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z2" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA2" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="Z2" s="52" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA2" s="14" t="s">
+      <c r="AB2" s="14" t="s">
         <v>51</v>
-      </c>
-      <c r="AB2" s="14" t="s">
-        <v>52</v>
       </c>
       <c r="AC2" s="14" t="s">
         <v>14</v>
       </c>
       <c r="AD2" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AE2" s="14" t="s">
         <v>33</v>
@@ -1250,7 +1248,7 @@
         <v>38</v>
       </c>
       <c r="AK2" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AL2" s="14" t="s">
         <v>37</v>
@@ -1258,16 +1256,18 @@
       <c r="AM2" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="AN2" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="AO2" s="40" t="s">
+      <c r="AN2" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO2" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP2" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="AP2" s="41" t="s">
-        <v>65</v>
-      </c>
-      <c r="AQ2" s="2"/>
+      <c r="AQ2" s="32" t="s">
+        <v>73</v>
+      </c>
       <c r="AR2" s="2"/>
       <c r="AS2" s="2"/>
       <c r="AT2" s="2"/>
@@ -1307,18 +1307,18 @@
       <c r="CB2" s="1"/>
       <c r="CC2" s="1"/>
     </row>
-    <row r="3" spans="1:81" s="47" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:81" s="38" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="C3" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="D3" s="19" t="s">
         <v>68</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>69</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3" s="19"/>
@@ -1326,16 +1326,16 @@
         <v>42</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="44" t="s">
+      <c r="J3" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49" t="s">
+      <c r="K3" s="40"/>
+      <c r="L3" s="40" t="s">
         <v>0</v>
       </c>
       <c r="M3" s="26" t="s">
@@ -1372,17 +1372,17 @@
       <c r="X3" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="Y3" s="53" t="s">
+      <c r="Y3" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="Z3" s="53" t="s">
+      <c r="Z3" s="44" t="s">
         <v>19</v>
       </c>
       <c r="AA3" s="27" t="s">
         <v>30</v>
       </c>
       <c r="AB3" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AC3" s="27" t="s">
         <v>0</v>
@@ -1415,54 +1415,54 @@
         <v>36</v>
       </c>
       <c r="AM3" s="28"/>
-      <c r="AN3" s="45" t="s">
+      <c r="AN3" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO3" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP3" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="AO3" s="42" t="s">
-        <v>72</v>
-      </c>
-      <c r="AP3" s="43" t="s">
-        <v>73</v>
-      </c>
-      <c r="AQ3" s="46"/>
-      <c r="AR3" s="46"/>
-      <c r="AS3" s="46"/>
-      <c r="AT3" s="46"/>
-      <c r="AU3" s="46"/>
-      <c r="AV3" s="46"/>
-      <c r="AW3" s="46"/>
-      <c r="AX3" s="46"/>
-      <c r="AY3" s="46"/>
-      <c r="AZ3" s="46"/>
-      <c r="BA3" s="46"/>
-      <c r="BB3" s="46"/>
-      <c r="BC3" s="46"/>
-      <c r="BD3" s="46"/>
-      <c r="BE3" s="46"/>
-      <c r="BF3" s="46"/>
-      <c r="BG3" s="46"/>
-      <c r="BH3" s="46"/>
-      <c r="BI3" s="46"/>
-      <c r="BJ3" s="46"/>
-      <c r="BK3" s="46"/>
-      <c r="BL3" s="46"/>
-      <c r="BM3" s="46"/>
-      <c r="BN3" s="46"/>
-      <c r="BO3" s="46"/>
-      <c r="BP3" s="46"/>
-      <c r="BQ3" s="46"/>
-      <c r="BR3" s="46"/>
-      <c r="BS3" s="46"/>
-      <c r="BT3" s="46"/>
-      <c r="BU3" s="46"/>
-      <c r="BV3" s="46"/>
-      <c r="BW3" s="46"/>
-      <c r="BX3" s="46"/>
-      <c r="BY3" s="46"/>
-      <c r="BZ3" s="45"/>
-      <c r="CA3" s="45"/>
-      <c r="CB3" s="45"/>
-      <c r="CC3" s="45"/>
+      <c r="AQ3" s="34"/>
+      <c r="AR3" s="37"/>
+      <c r="AS3" s="37"/>
+      <c r="AT3" s="37"/>
+      <c r="AU3" s="37"/>
+      <c r="AV3" s="37"/>
+      <c r="AW3" s="37"/>
+      <c r="AX3" s="37"/>
+      <c r="AY3" s="37"/>
+      <c r="AZ3" s="37"/>
+      <c r="BA3" s="37"/>
+      <c r="BB3" s="37"/>
+      <c r="BC3" s="37"/>
+      <c r="BD3" s="37"/>
+      <c r="BE3" s="37"/>
+      <c r="BF3" s="37"/>
+      <c r="BG3" s="37"/>
+      <c r="BH3" s="37"/>
+      <c r="BI3" s="37"/>
+      <c r="BJ3" s="37"/>
+      <c r="BK3" s="37"/>
+      <c r="BL3" s="37"/>
+      <c r="BM3" s="37"/>
+      <c r="BN3" s="37"/>
+      <c r="BO3" s="37"/>
+      <c r="BP3" s="37"/>
+      <c r="BQ3" s="37"/>
+      <c r="BR3" s="37"/>
+      <c r="BS3" s="37"/>
+      <c r="BT3" s="37"/>
+      <c r="BU3" s="37"/>
+      <c r="BV3" s="37"/>
+      <c r="BW3" s="37"/>
+      <c r="BX3" s="37"/>
+      <c r="BY3" s="37"/>
+      <c r="BZ3" s="36"/>
+      <c r="CA3" s="36"/>
+      <c r="CB3" s="36"/>
+      <c r="CC3" s="36"/>
     </row>
     <row r="4" spans="1:81" x14ac:dyDescent="0.15">
       <c r="A4" s="22"/>
@@ -1506,8 +1506,8 @@
       <c r="AM4" s="22"/>
       <c r="AN4" s="21"/>
       <c r="AO4" s="22"/>
-      <c r="AP4" s="50"/>
-      <c r="AQ4" s="23"/>
+      <c r="AP4" s="23"/>
+      <c r="AQ4" s="41"/>
       <c r="AR4" s="23"/>
       <c r="AS4" s="23"/>
       <c r="AT4" s="23"/>
@@ -1552,7 +1552,7 @@
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="K1:S1"/>
     <mergeCell ref="T1:X1"/>
-    <mergeCell ref="Y1:AP1"/>
+    <mergeCell ref="Y1:AQ1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update accessioning template docs
</commit_message>
<xml_diff>
--- a/docs/public/help/help_linked_docs/accessioning_template_extended.xlsx
+++ b/docs/public/help/help_linked_docs/accessioning_template_extended.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drioux/CGAP/cgap-portal/docs/public/help/help_linked_docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drioux/CGAP/cgap-portal-2/docs/public/help/help_linked_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95890A0-8CCF-C148-8E8F-FF19BF7A2C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62FC312-2D4F-4A49-8B6B-8D2BA3FDFF5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="28800" windowHeight="14860" xr2:uid="{FB0E66EA-1423-4875-8AFB-50DDC911B1EB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="77">
   <si>
     <t>dd/mm/yyyy</t>
   </si>
@@ -250,6 +250,12 @@
   </si>
   <si>
     <t>Individual ID*</t>
+  </si>
+  <si>
+    <t>Variant Type</t>
+  </si>
+  <si>
+    <t>SNV, SV, CNV</t>
   </si>
 </sst>
 </file>
@@ -578,7 +584,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -692,6 +698,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1014,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23985C4D-01B8-468F-8F7A-3E2DDE3ABF1C}">
-  <dimension ref="A1:CC4"/>
+  <dimension ref="A1:CD4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AQ9" sqref="AQ9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1040,16 +1049,17 @@
     <col min="40" max="40" width="14.33203125" style="5" customWidth="1"/>
     <col min="41" max="41" width="12.6640625" style="4" customWidth="1"/>
     <col min="42" max="42" width="16" style="7" customWidth="1"/>
-    <col min="43" max="43" width="16" style="42" customWidth="1"/>
-    <col min="44" max="77" width="16" style="7" customWidth="1"/>
-    <col min="78" max="78" width="14.5" style="4" customWidth="1"/>
-    <col min="79" max="79" width="15.5" style="4" customWidth="1"/>
-    <col min="80" max="80" width="14.33203125" style="4" customWidth="1"/>
-    <col min="81" max="81" width="16.5" style="4" customWidth="1"/>
-    <col min="82" max="16384" width="9.1640625" style="8"/>
+    <col min="43" max="43" width="16" style="4" customWidth="1"/>
+    <col min="44" max="44" width="16" style="42" customWidth="1"/>
+    <col min="45" max="78" width="16" style="7" customWidth="1"/>
+    <col min="79" max="79" width="14.5" style="4" customWidth="1"/>
+    <col min="80" max="80" width="15.5" style="4" customWidth="1"/>
+    <col min="81" max="81" width="14.33203125" style="4" customWidth="1"/>
+    <col min="82" max="82" width="16.5" style="4" customWidth="1"/>
+    <col min="83" max="16384" width="9.1640625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:81" s="3" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:82" s="3" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="45" t="s">
         <v>3</v>
       </c>
@@ -1098,8 +1108,8 @@
       <c r="AN1" s="47"/>
       <c r="AO1" s="47"/>
       <c r="AP1" s="47"/>
-      <c r="AQ1" s="50"/>
-      <c r="AR1" s="15"/>
+      <c r="AQ1" s="47"/>
+      <c r="AR1" s="50"/>
       <c r="AS1" s="15"/>
       <c r="AT1" s="15"/>
       <c r="AU1" s="15"/>
@@ -1133,12 +1143,13 @@
       <c r="BW1" s="15"/>
       <c r="BX1" s="15"/>
       <c r="BY1" s="15"/>
-      <c r="BZ1" s="16"/>
+      <c r="BZ1" s="15"/>
       <c r="CA1" s="16"/>
       <c r="CB1" s="16"/>
       <c r="CC1" s="16"/>
+      <c r="CD1" s="16"/>
     </row>
-    <row r="2" spans="1:81" s="9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:82" s="9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>48</v>
       </c>
@@ -1265,10 +1276,12 @@
       <c r="AP2" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="AQ2" s="32" t="s">
+      <c r="AQ2" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR2" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="AR2" s="2"/>
       <c r="AS2" s="2"/>
       <c r="AT2" s="2"/>
       <c r="AU2" s="2"/>
@@ -1302,12 +1315,13 @@
       <c r="BW2" s="2"/>
       <c r="BX2" s="2"/>
       <c r="BY2" s="2"/>
-      <c r="BZ2" s="1"/>
+      <c r="BZ2" s="2"/>
       <c r="CA2" s="1"/>
       <c r="CB2" s="1"/>
       <c r="CC2" s="1"/>
+      <c r="CD2" s="1"/>
     </row>
-    <row r="3" spans="1:81" s="38" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:82" s="38" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>65</v>
       </c>
@@ -1424,8 +1438,10 @@
       <c r="AP3" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="AQ3" s="34"/>
-      <c r="AR3" s="37"/>
+      <c r="AQ3" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="AR3" s="34"/>
       <c r="AS3" s="37"/>
       <c r="AT3" s="37"/>
       <c r="AU3" s="37"/>
@@ -1459,12 +1475,13 @@
       <c r="BW3" s="37"/>
       <c r="BX3" s="37"/>
       <c r="BY3" s="37"/>
-      <c r="BZ3" s="36"/>
+      <c r="BZ3" s="37"/>
       <c r="CA3" s="36"/>
       <c r="CB3" s="36"/>
       <c r="CC3" s="36"/>
+      <c r="CD3" s="36"/>
     </row>
-    <row r="4" spans="1:81" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:82" x14ac:dyDescent="0.15">
       <c r="A4" s="22"/>
       <c r="B4" s="23"/>
       <c r="C4" s="21"/>
@@ -1507,8 +1524,8 @@
       <c r="AN4" s="21"/>
       <c r="AO4" s="22"/>
       <c r="AP4" s="23"/>
-      <c r="AQ4" s="41"/>
-      <c r="AR4" s="23"/>
+      <c r="AQ4" s="22"/>
+      <c r="AR4" s="41"/>
       <c r="AS4" s="23"/>
       <c r="AT4" s="23"/>
       <c r="AU4" s="23"/>
@@ -1542,17 +1559,18 @@
       <c r="BW4" s="23"/>
       <c r="BX4" s="23"/>
       <c r="BY4" s="23"/>
-      <c r="BZ4" s="22"/>
+      <c r="BZ4" s="23"/>
       <c r="CA4" s="22"/>
       <c r="CB4" s="22"/>
       <c r="CC4" s="22"/>
+      <c r="CD4" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="K1:S1"/>
     <mergeCell ref="T1:X1"/>
-    <mergeCell ref="Y1:AQ1"/>
+    <mergeCell ref="Y1:AR1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add Tags column to extended accession spreadsheets
</commit_message>
<xml_diff>
--- a/docs/public/help/help_linked_docs/accessioning_template_extended.xlsx
+++ b/docs/public/help/help_linked_docs/accessioning_template_extended.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drioux/CGAP/cgap-portal-2/docs/public/help/help_linked_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62FC312-2D4F-4A49-8B6B-8D2BA3FDFF5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A4B69F-5ED7-4A48-A3DC-08B324317432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="28800" windowHeight="14860" xr2:uid="{FB0E66EA-1423-4875-8AFB-50DDC911B1EB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="78">
   <si>
     <t>dd/mm/yyyy</t>
   </si>
@@ -256,6 +256,9 @@
   </si>
   <si>
     <t>SNV, SV, CNV</t>
+  </si>
+  <si>
+    <t>Tags</t>
   </si>
 </sst>
 </file>
@@ -678,6 +681,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -698,9 +704,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -727,7 +730,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1015,7 +1018,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1023,10 +1026,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23985C4D-01B8-468F-8F7A-3E2DDE3ABF1C}">
-  <dimension ref="A1:CD4"/>
+  <dimension ref="A1:CE4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AQ9" sqref="AQ9"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AN2" sqref="AN2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1045,72 +1048,72 @@
     <col min="26" max="35" width="16" style="7" customWidth="1"/>
     <col min="36" max="37" width="14.5" style="4" customWidth="1"/>
     <col min="38" max="38" width="15.5" style="4" customWidth="1"/>
-    <col min="39" max="39" width="14.33203125" style="4" customWidth="1"/>
-    <col min="40" max="40" width="14.33203125" style="5" customWidth="1"/>
-    <col min="41" max="41" width="12.6640625" style="4" customWidth="1"/>
-    <col min="42" max="42" width="16" style="7" customWidth="1"/>
-    <col min="43" max="43" width="16" style="4" customWidth="1"/>
-    <col min="44" max="44" width="16" style="42" customWidth="1"/>
-    <col min="45" max="78" width="16" style="7" customWidth="1"/>
-    <col min="79" max="79" width="14.5" style="4" customWidth="1"/>
-    <col min="80" max="80" width="15.5" style="4" customWidth="1"/>
-    <col min="81" max="81" width="14.33203125" style="4" customWidth="1"/>
-    <col min="82" max="82" width="16.5" style="4" customWidth="1"/>
-    <col min="83" max="16384" width="9.1640625" style="8"/>
+    <col min="39" max="40" width="14.33203125" style="4" customWidth="1"/>
+    <col min="41" max="41" width="14.33203125" style="5" customWidth="1"/>
+    <col min="42" max="42" width="12.6640625" style="4" customWidth="1"/>
+    <col min="43" max="43" width="16" style="7" customWidth="1"/>
+    <col min="44" max="44" width="16" style="4" customWidth="1"/>
+    <col min="45" max="45" width="16" style="42" customWidth="1"/>
+    <col min="46" max="79" width="16" style="7" customWidth="1"/>
+    <col min="80" max="80" width="14.5" style="4" customWidth="1"/>
+    <col min="81" max="81" width="15.5" style="4" customWidth="1"/>
+    <col min="82" max="82" width="14.33203125" style="4" customWidth="1"/>
+    <col min="83" max="83" width="16.5" style="4" customWidth="1"/>
+    <col min="84" max="16384" width="9.1640625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:82" s="3" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:83" s="3" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="48"/>
-      <c r="T1" s="49" t="s">
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="48"/>
+      <c r="S1" s="49"/>
+      <c r="T1" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="U1" s="47"/>
-      <c r="V1" s="47"/>
-      <c r="W1" s="47"/>
-      <c r="X1" s="50"/>
-      <c r="Y1" s="51" t="s">
+      <c r="U1" s="48"/>
+      <c r="V1" s="48"/>
+      <c r="W1" s="48"/>
+      <c r="X1" s="51"/>
+      <c r="Y1" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="Z1" s="47"/>
-      <c r="AA1" s="47"/>
-      <c r="AB1" s="47"/>
-      <c r="AC1" s="47"/>
-      <c r="AD1" s="47"/>
-      <c r="AE1" s="47"/>
-      <c r="AF1" s="47"/>
-      <c r="AG1" s="47"/>
-      <c r="AH1" s="47"/>
-      <c r="AI1" s="47"/>
-      <c r="AJ1" s="47"/>
-      <c r="AK1" s="47"/>
-      <c r="AL1" s="47"/>
-      <c r="AM1" s="47"/>
-      <c r="AN1" s="47"/>
-      <c r="AO1" s="47"/>
-      <c r="AP1" s="47"/>
-      <c r="AQ1" s="47"/>
-      <c r="AR1" s="50"/>
-      <c r="AS1" s="15"/>
+      <c r="Z1" s="48"/>
+      <c r="AA1" s="48"/>
+      <c r="AB1" s="48"/>
+      <c r="AC1" s="48"/>
+      <c r="AD1" s="48"/>
+      <c r="AE1" s="48"/>
+      <c r="AF1" s="48"/>
+      <c r="AG1" s="48"/>
+      <c r="AH1" s="48"/>
+      <c r="AI1" s="48"/>
+      <c r="AJ1" s="48"/>
+      <c r="AK1" s="48"/>
+      <c r="AL1" s="48"/>
+      <c r="AM1" s="48"/>
+      <c r="AN1" s="48"/>
+      <c r="AO1" s="48"/>
+      <c r="AP1" s="48"/>
+      <c r="AQ1" s="48"/>
+      <c r="AR1" s="48"/>
+      <c r="AS1" s="51"/>
       <c r="AT1" s="15"/>
       <c r="AU1" s="15"/>
       <c r="AV1" s="15"/>
@@ -1144,12 +1147,13 @@
       <c r="BX1" s="15"/>
       <c r="BY1" s="15"/>
       <c r="BZ1" s="15"/>
-      <c r="CA1" s="16"/>
+      <c r="CA1" s="15"/>
       <c r="CB1" s="16"/>
       <c r="CC1" s="16"/>
       <c r="CD1" s="16"/>
+      <c r="CE1" s="16"/>
     </row>
-    <row r="2" spans="1:82" s="9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:83" s="9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>48</v>
       </c>
@@ -1267,22 +1271,24 @@
       <c r="AM2" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="AN2" s="30" t="s">
+      <c r="AN2" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="AO2" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="AO2" s="31" t="s">
+      <c r="AP2" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="AP2" s="31" t="s">
+      <c r="AQ2" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="AQ2" s="52" t="s">
+      <c r="AR2" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="AR2" s="32" t="s">
+      <c r="AS2" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="AS2" s="2"/>
       <c r="AT2" s="2"/>
       <c r="AU2" s="2"/>
       <c r="AV2" s="2"/>
@@ -1316,12 +1322,13 @@
       <c r="BX2" s="2"/>
       <c r="BY2" s="2"/>
       <c r="BZ2" s="2"/>
-      <c r="CA2" s="1"/>
+      <c r="CA2" s="2"/>
       <c r="CB2" s="1"/>
       <c r="CC2" s="1"/>
       <c r="CD2" s="1"/>
+      <c r="CE2" s="1"/>
     </row>
-    <row r="3" spans="1:82" s="38" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:83" s="38" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>65</v>
       </c>
@@ -1429,20 +1436,22 @@
         <v>36</v>
       </c>
       <c r="AM3" s="28"/>
-      <c r="AN3" s="36" t="s">
+      <c r="AN3" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="AO3" s="33" t="s">
+      <c r="AO3" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="AP3" s="37" t="s">
+      <c r="AP3" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="AQ3" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="AQ3" s="33" t="s">
+      <c r="AR3" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="AR3" s="34"/>
-      <c r="AS3" s="37"/>
+      <c r="AS3" s="34"/>
       <c r="AT3" s="37"/>
       <c r="AU3" s="37"/>
       <c r="AV3" s="37"/>
@@ -1476,12 +1485,13 @@
       <c r="BX3" s="37"/>
       <c r="BY3" s="37"/>
       <c r="BZ3" s="37"/>
-      <c r="CA3" s="36"/>
+      <c r="CA3" s="37"/>
       <c r="CB3" s="36"/>
       <c r="CC3" s="36"/>
       <c r="CD3" s="36"/>
+      <c r="CE3" s="36"/>
     </row>
-    <row r="4" spans="1:82" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:83" x14ac:dyDescent="0.15">
       <c r="A4" s="22"/>
       <c r="B4" s="23"/>
       <c r="C4" s="21"/>
@@ -1521,12 +1531,12 @@
       <c r="AK4" s="22"/>
       <c r="AL4" s="22"/>
       <c r="AM4" s="22"/>
-      <c r="AN4" s="21"/>
-      <c r="AO4" s="22"/>
-      <c r="AP4" s="23"/>
-      <c r="AQ4" s="22"/>
-      <c r="AR4" s="41"/>
-      <c r="AS4" s="23"/>
+      <c r="AN4" s="22"/>
+      <c r="AO4" s="21"/>
+      <c r="AP4" s="22"/>
+      <c r="AQ4" s="23"/>
+      <c r="AR4" s="22"/>
+      <c r="AS4" s="41"/>
       <c r="AT4" s="23"/>
       <c r="AU4" s="23"/>
       <c r="AV4" s="23"/>
@@ -1560,17 +1570,18 @@
       <c r="BX4" s="23"/>
       <c r="BY4" s="23"/>
       <c r="BZ4" s="23"/>
-      <c r="CA4" s="22"/>
+      <c r="CA4" s="23"/>
       <c r="CB4" s="22"/>
       <c r="CC4" s="22"/>
       <c r="CD4" s="22"/>
+      <c r="CE4" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="K1:S1"/>
     <mergeCell ref="T1:X1"/>
-    <mergeCell ref="Y1:AR1"/>
+    <mergeCell ref="Y1:AS1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>